<commit_message>
seperate two boards' design document
</commit_message>
<xml_diff>
--- a/HISTORY/design_flow.xlsx
+++ b/HISTORY/design_flow.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\work\dsp\workspace\F2812_SAMPLER\HISTORY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F4AF3D-29E6-4188-B75A-FE79E33A3827}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95730F06-3F21-40E4-A12F-7C96E27390B4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RS422 驱动" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="SAMPLER Architecture" sheetId="3" r:id="rId2"/>
+    <sheet name="DISPLAY Architecture" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -2429,6 +2430,4002 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>213360</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>41413</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7511A55-CDCF-4B2D-BE72-D82F8D4BC274}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="822960" y="1264920"/>
+          <a:ext cx="2887980" cy="1755913"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>F2812</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="zh-CN">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>144781</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10BB67D3-6322-48D7-9725-915E7342E6A9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2583180" y="1371601"/>
+          <a:ext cx="1188720" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>SCI-A</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="zh-CN">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>449580</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>502920</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>30479</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23AB2031-1E60-4220-A043-960D0BCBC2B3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1059180" y="3512820"/>
+          <a:ext cx="1882140" cy="1775459"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>FPGA</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="zh-CN">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>563880</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>160021</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>213360</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>15241</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Rectangle 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93169B1E-47E4-44CF-ADB5-970A426E0064}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1173480" y="3840481"/>
+          <a:ext cx="868680" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>SRAM</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="zh-CN">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>403860</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>53341</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>548640</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>83821</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Rectangle 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E0A871E-09F2-43C5-817F-7216D537E441}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2232660" y="3558541"/>
+          <a:ext cx="754380" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>RS422</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="zh-CN">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>175260</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>312420</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectangle 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7EEC3127-5C75-4F0B-BBC1-581942063C0F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4442460" y="1219200"/>
+          <a:ext cx="1356360" cy="2849879"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>Externl BOARD</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="zh-CN">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>365760</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>60959</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rectangle 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0671E8B-32FA-4E1B-91DD-1C923528B1B8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4373880" y="3337560"/>
+          <a:ext cx="868680" cy="579119"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="r" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>I/O Switches</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="zh-CN">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>365760</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>68581</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Rectangle 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64A56C94-95D9-4FF8-8093-6F8B5926550D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4373880" y="2491741"/>
+          <a:ext cx="868680" cy="556260"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>RS422 </a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="zh-CN">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>297180</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>83819</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rectangle 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{701BCE5C-3A08-4CC6-A015-CDA27A4B888D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2125980" y="4411980"/>
+          <a:ext cx="868680" cy="579119"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>I/O Switches</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="zh-CN">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>548640</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>106681</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Rectangle 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6019C5B6-EA49-4BCF-9915-7019A8A61C44}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1181100" y="2705101"/>
+          <a:ext cx="586740" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>CS0&amp;1</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="zh-CN">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>312420</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>68581</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>99061</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Rectangle 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA81E4C1-15DF-4B18-9EC0-A4FDD6FF85D7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2141220" y="2697481"/>
+          <a:ext cx="586740" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>CS2</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="zh-CN">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>548640</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>140971</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>68581</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Connector: Elbow 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE4A3307-E4B1-420E-AA05-CD8DF27649B7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="6" idx="3"/>
+          <a:endCxn id="10" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2987040" y="2769871"/>
+          <a:ext cx="1386840" cy="979170"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 70330"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="dk1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="arrow" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Connector: Elbow 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2FC8993D-807C-468B-8CAC-7C44CC6BA4DE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="11" idx="3"/>
+          <a:endCxn id="9" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2994660" y="3627120"/>
+          <a:ext cx="1379220" cy="1074420"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 79834"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="dk1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="arrow" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>320040</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Straight Connector 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A0147CE-75BC-4C1B-A3BB-BFBA4E96EB74}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3977640" y="4114800"/>
+          <a:ext cx="236220" cy="144780"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>449580</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>106682</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>255270</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Connector: Elbow 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E77FF489-CD89-4706-8798-3D58BDA7F07E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="1"/>
+          <a:endCxn id="12" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipH="1">
+          <a:off x="1059180" y="3086102"/>
+          <a:ext cx="415290" cy="1314449"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector4">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -55046"/>
+            <a:gd name="adj2" fmla="val 83768"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="dk1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="arrow" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>171451</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>99061</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>605791</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Connector: Elbow 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1ACF7245-6ABF-457B-975A-6EE205A8287E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="0"/>
+          <a:endCxn id="13" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="2000251" y="3078481"/>
+          <a:ext cx="434339" cy="434340"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="dk1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="arrow" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>99060</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>144781</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="Rectangle 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{06CC8614-E8CA-458D-AE95-7248DD93B082}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1348740" y="464821"/>
+          <a:ext cx="1188720" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>F-RAM</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="zh-CN">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>327660</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>426720</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>7621</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="Rectangle 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30D44925-47F3-4872-8996-86DC6A908218}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1546860" y="1203961"/>
+          <a:ext cx="708660" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>SPI</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="zh-CN">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>72390</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>129541</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>99060</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Connector: Elbow 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9E876F7-EE9E-4736-BBF9-BD175E7690A7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="21" idx="0"/>
+          <a:endCxn id="20" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="1945005" y="611506"/>
+          <a:ext cx="548640" cy="636270"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector4">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 32639"/>
+            <a:gd name="adj2" fmla="val 135928"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="dk1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="arrow" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>167640</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>403860</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Straight Connector 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B063ECAA-7285-4583-B118-6E80E1060B5A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3825240" y="3169920"/>
+          <a:ext cx="236220" cy="144780"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>373380</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>30481</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>60961</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="Rectangle 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FB5EE2F-E1C8-4871-B686-6583F225299D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3421380" y="381001"/>
+          <a:ext cx="1188720" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>Console</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="zh-CN">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>60961</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>358140</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>144781</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Connector: Elbow 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E17FD74-05E3-49C1-852A-3CFB2707A9DD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="0"/>
+          <a:endCxn id="24" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="3291840" y="647701"/>
+          <a:ext cx="609600" cy="838200"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="dk1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="arrow" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>144781</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>312420</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="28" name="Rectangle 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0E3C33F-E710-4472-8603-C0F5786BAEEF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2324100" y="5052061"/>
+          <a:ext cx="426720" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>SPI</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="zh-CN">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>464820</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>68581</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="Rectangle 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C1EFFB7-5E12-412C-9365-E661488FA4D6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3543300" y="5120641"/>
+          <a:ext cx="1188720" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>ADS1248</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="zh-CN">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>144781</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="30" name="Rectangle 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9197C74C-D5C3-4385-8D20-326F58F2EBEA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3535680" y="5753101"/>
+          <a:ext cx="1188720" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>AD5684</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="zh-CN">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>99060</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>480060</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="31" name="Connector: Elbow 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A80C14CD-A754-4967-AE97-1C8942882D8C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="28" idx="2"/>
+          <a:endCxn id="29" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="3181350" y="4476751"/>
+          <a:ext cx="312420" cy="1600200"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector5">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -73171"/>
+            <a:gd name="adj2" fmla="val 38095"/>
+            <a:gd name="adj3" fmla="val 173171"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="dk1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="arrow" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>167640</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>129541</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>160021</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="36" name="Rectangle 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF0A80DD-8E90-48FE-A289-D314AB587AB5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1386840" y="5036821"/>
+          <a:ext cx="426720" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>SPI</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="zh-CN">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>160021</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>160021</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="38" name="Connector: Elbow 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{100C59FE-88C5-4CC8-915D-C699A9BA32CF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="36" idx="2"/>
+          <a:endCxn id="30" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="2305050" y="4712971"/>
+          <a:ext cx="525780" cy="1935480"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="dk1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="arrow" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>213360</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>41413</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E71D24B-0879-43EC-8B71-459E3613AD0D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2651760" y="1264920"/>
+          <a:ext cx="2887980" cy="1755913"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>F2812</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="zh-CN">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>144781</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4F859C5-D19D-4F3C-8655-CD1289AFD71E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4411980" y="1371601"/>
+          <a:ext cx="1188720" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>SCI-B</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="zh-CN">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>449580</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>502920</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>30479</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5492821E-EAA4-4472-B4E6-486C2C4FC5E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2887980" y="3512820"/>
+          <a:ext cx="1882140" cy="1775459"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>FPGA</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="zh-CN">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>563880</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>160021</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>213360</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>15241</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Rectangle 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5D38749-7427-4357-8F5C-B55D1C013C29}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3002280" y="3840481"/>
+          <a:ext cx="868680" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>SRAM</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="zh-CN">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>403860</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>53341</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>548640</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>83821</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Rectangle 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8AD4581-C577-4A97-A6EA-DD5283AB032A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4061460" y="3558541"/>
+          <a:ext cx="754380" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>RS422</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="zh-CN">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>175260</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>312420</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectangle 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11A3D8A3-81FA-4480-B342-2FF16B91695A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6271260" y="1219200"/>
+          <a:ext cx="1356360" cy="2849879"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>DISPLAY</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t> BOARD</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="zh-CN">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>365760</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>30481</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Rectangle 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37564984-F19F-47A9-AB90-52382BAFCB73}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6202680" y="1752601"/>
+          <a:ext cx="868680" cy="556260"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>RS422 Channel</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t> 0</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="zh-CN">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>365760</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>60959</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rectangle 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18F17802-E3E6-41EB-B559-8602BB5BD47C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6202680" y="3337560"/>
+          <a:ext cx="868680" cy="579119"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="r" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>I/O Switches</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="zh-CN">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>365760</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>68581</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Rectangle 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13AD45A0-FCA6-434B-A1F2-4652E2EA7020}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6202680" y="2491741"/>
+          <a:ext cx="868680" cy="556260"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>RS422 Channel</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t> 1</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="zh-CN">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>297180</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>83819</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rectangle 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27B9F373-7EF5-4178-8BF9-8D201C0F9F2D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3954780" y="4411980"/>
+          <a:ext cx="868680" cy="579119"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>I/O Switches</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="zh-CN">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>548640</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>106681</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Rectangle 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7E62823-EE6B-47CD-966B-1E3C703104CB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3009900" y="2705101"/>
+          <a:ext cx="586740" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>CS0&amp;1</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="zh-CN">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>312420</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>68581</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>99061</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Rectangle 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A7F6060-984A-46A2-ADBE-FAAE1FED2AF3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3970020" y="2697481"/>
+          <a:ext cx="586740" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>CS2</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="zh-CN">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>160021</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>102871</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Connector: Elbow 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BABA21A-62DF-484B-84CF-27A2310E9467}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="3"/>
+          <a:endCxn id="8" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5600700" y="1562101"/>
+          <a:ext cx="601980" cy="468630"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="dk1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="arrow" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>548640</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>140971</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>68581</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Connector: Elbow 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A89D046-1163-494B-88EF-BBC374601ADB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="6" idx="3"/>
+          <a:endCxn id="10" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4815840" y="2769871"/>
+          <a:ext cx="1386840" cy="979170"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 70330"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="dk1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="arrow" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Connector: Elbow 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6B6ED4D-CE04-4B0F-9282-6BD5FE5AA04F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="11" idx="3"/>
+          <a:endCxn id="9" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4823460" y="3627120"/>
+          <a:ext cx="1379220" cy="1074420"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 79834"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="dk1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="arrow" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>320040</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Straight Connector 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17C8238F-365A-4A00-B21B-9306E580ED5B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5806440" y="4114800"/>
+          <a:ext cx="236220" cy="144780"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>449580</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>106682</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>255270</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="27" name="Connector: Elbow 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4DAEB64-0FF4-4B8F-97B0-D9B529B44F4A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="1"/>
+          <a:endCxn id="12" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipH="1">
+          <a:off x="2887980" y="3086102"/>
+          <a:ext cx="415290" cy="1314449"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector4">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -55046"/>
+            <a:gd name="adj2" fmla="val 83768"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="dk1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="arrow" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>171451</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>99061</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>605791</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="30" name="Connector: Elbow 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8C418B0-E470-41BF-B839-A69894725035}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="0"/>
+          <a:endCxn id="13" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="3829051" y="3078481"/>
+          <a:ext cx="434339" cy="434340"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="dk1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="arrow" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>99060</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>68580</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="39" name="Rectangle 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54ACEB47-0F4B-48D0-9006-A9F79094695A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1318260" y="1226820"/>
+          <a:ext cx="1188720" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>SCI-A</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="zh-CN">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>426720</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>396240</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="40" name="Rectangle 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{632404CC-A986-45B4-8D61-C4884B57DF2A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2255520" y="464820"/>
+          <a:ext cx="1188720" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>Console</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="zh-CN">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>411480</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="41" name="Connector: Elbow 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{268A6FC4-E3C6-47C8-8145-D7D7850C144A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="39" idx="0"/>
+          <a:endCxn id="40" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="2190750" y="567690"/>
+          <a:ext cx="381000" cy="937260"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="dk1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="arrow" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2697,8 +6694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A23" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView showGridLines="0" topLeftCell="A23" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2714,14 +6711,35 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BECADCDE-60A2-45F0-A5EF-87E9633833F7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{066DB759-BAF9-4B6F-AA9B-9BDFDB7573C3}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BECADCDE-60A2-45F0-A5EF-87E9633833F7}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>